<commit_message>
Reading in default data in new format
</commit_message>
<xml_diff>
--- a/applications/master/data/national/master_input.xlsx
+++ b/applications/master/data/national/master_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{72652FDC-77F7-BF46-9629-F8DB58CAB3E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{3FA8A740-9914-534F-B67E-D74E338CFEE8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="-19800" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13020" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="961" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -8944,7 +8944,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
@@ -11167,7 +11167,7 @@
   </sheetPr>
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Changed refs to match the new strings in spreadsheet, variable name changes
</commit_message>
<xml_diff>
--- a/applications/master/data/national/master_input.xlsx
+++ b/applications/master/data/national/master_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5E9B6A32-1CEB-534B-AE95-A154DB98B182}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{F4C5A40D-73DC-164A-A40B-C85FB21CAE30}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="961" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4183,7 +4183,7 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
@@ -4565,7 +4565,7 @@
   </sheetPr>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -5422,7 +5422,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6073,8 +6073,8 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6993,12 +6993,12 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
-    <tabColor rgb="FF007600"/>
+    <tabColor theme="0" tint="-0.34998626667073579"/>
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7027,19 +7027,24 @@
       <c r="A2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="40">
+        <f>'Baseline year population inputs'!C39</f>
         <v>2.4300000000000002</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="40">
+        <f>'Baseline year population inputs'!C40</f>
         <v>2.4300000000000002</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="40">
+        <f>'Baseline year population inputs'!C41</f>
         <v>3.71</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="40">
+        <f>'Baseline year population inputs'!C42</f>
         <v>3</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="40">
+        <f>'Baseline year population inputs'!C43</f>
         <v>1.92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A host of updates to make model compatible with the Project class, deleted old files
</commit_message>
<xml_diff>
--- a/applications/master/data/national/master_input.xlsx
+++ b/applications/master/data/national/master_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D55B6C65-5361-A74E-8DD2-46797FAF5C0F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{50A48E2E-96A0-C347-8378-5EDD1535F14F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="Programs family planning" sheetId="54" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="abortion">'Baseline year population inputs'!$C$26</definedName>
+    <definedName name="abortion">'Baseline year population inputs'!$C$29</definedName>
     <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$8</definedName>
     <definedName name="food_insecure">'Baseline year population inputs'!$C$3</definedName>
     <definedName name="frac_children_health_facility">'Baseline year population inputs'!$C$7</definedName>
@@ -49,18 +49,18 @@
     <definedName name="frac_SAMtoMAM">'Baseline year population inputs'!$C$49</definedName>
     <definedName name="frac_subsistence_farming">'Baseline year population inputs'!$C$11</definedName>
     <definedName name="frac_wheat">'Baseline year population inputs'!$C$13</definedName>
-    <definedName name="infant_mortality">'Baseline year population inputs'!$C$29</definedName>
+    <definedName name="infant_mortality">'Baseline year population inputs'!$C$26</definedName>
     <definedName name="iron_deficiency_anaemia">'Baseline year population inputs'!$C$47</definedName>
-    <definedName name="maternal_mortality">'Baseline year population inputs'!$C$25</definedName>
-    <definedName name="neonatal_mortality">'Baseline year population inputs'!$C$28</definedName>
+    <definedName name="maternal_mortality">'Baseline year population inputs'!$C$28</definedName>
+    <definedName name="neonatal_mortality">'Baseline year population inputs'!$C$25</definedName>
     <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Baseline year population inputs'!$C$6</definedName>
     <definedName name="preterm_AGA">'Baseline year population inputs'!$C$34</definedName>
     <definedName name="preterm_SGA">'Baseline year population inputs'!$C$33</definedName>
     <definedName name="school_attendance">'Baseline year population inputs'!$C$5</definedName>
-    <definedName name="stillbirth">'Baseline year population inputs'!$C$27</definedName>
+    <definedName name="stillbirth">'Baseline year population inputs'!$C$30</definedName>
     <definedName name="term_AGA">'Baseline year population inputs'!$C$36</definedName>
     <definedName name="term_SGA">'Baseline year population inputs'!$C$35</definedName>
-    <definedName name="U5_mortality">'Baseline year population inputs'!$C$30</definedName>
+    <definedName name="U5_mortality">'Baseline year population inputs'!$C$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="215">
   <si>
     <t>year</t>
   </si>
@@ -609,9 +609,6 @@
     <t>Stillbirths (per 1,000 total births)</t>
   </si>
   <si>
-    <t>Maternal mortality (per 100,000 live births)</t>
-  </si>
-  <si>
     <t>Fraction of subsistence farming</t>
   </si>
   <si>
@@ -813,15 +810,9 @@
     <t>Children 0-5 months</t>
   </si>
   <si>
-    <t>Maternal (deaths per 100,000 births)</t>
-  </si>
-  <si>
     <t>Under five (deaths per 1,000 births)</t>
   </si>
   <si>
-    <t xml:space="preserve">Mortality </t>
-  </si>
-  <si>
     <t>Delayed cord clamping</t>
   </si>
   <si>
@@ -883,6 +874,12 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Maternal (deaths per 1,000 births)</t>
+  </si>
+  <si>
+    <t>Maternal mortality (per 1,000 live births)</t>
   </si>
 </sst>
 </file>
@@ -1813,7 +1810,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1948,13 +1945,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="8" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4138,8 +4130,8 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4151,13 +4143,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B1" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="C1" s="72" t="s">
-        <v>211</v>
+        <v>130</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4167,7 +4159,7 @@
     </row>
     <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="27">
         <v>0.36</v>
@@ -4175,7 +4167,7 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="26">
         <v>0.1</v>
@@ -4183,7 +4175,7 @@
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C5" s="26">
         <v>0.35199999999999998</v>
@@ -4191,7 +4183,7 @@
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C6" s="27">
         <v>0.5</v>
@@ -4199,7 +4191,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="27">
         <v>0.3</v>
@@ -4207,7 +4199,7 @@
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" s="27">
         <v>0.1</v>
@@ -4225,7 +4217,7 @@
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="26">
         <v>0.3</v>
@@ -4233,7 +4225,7 @@
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="26">
         <v>0.8</v>
@@ -4241,7 +4233,7 @@
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" s="26">
         <v>0.12</v>
@@ -4249,7 +4241,7 @@
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="26">
         <v>0.05</v>
@@ -4257,7 +4249,7 @@
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="29">
         <f>1-frac_rice-frac_wheat-frac_maize</f>
@@ -4269,12 +4261,12 @@
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="26">
         <v>0.29978973218277538</v>
@@ -4282,7 +4274,7 @@
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="26">
         <v>0.52556568434139284</v>
@@ -4290,7 +4282,7 @@
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="26">
         <v>0.16210210664201097</v>
@@ -4298,7 +4290,7 @@
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="30" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="26">
         <v>1.2542476833820825E-2</v>
@@ -4307,7 +4299,7 @@
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4318,63 +4310,63 @@
       <c r="C24" s="19"/>
     </row>
     <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="22" t="s">
-        <v>124</v>
+      <c r="B25" s="71" t="s">
+        <v>122</v>
       </c>
       <c r="C25" s="28">
-        <v>176</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="C26" s="26">
-        <v>0.13</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="C26" s="28">
+        <v>34.68</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="57" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="58">
-        <v>25.36</v>
-      </c>
+      <c r="B27" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C27" s="28">
+        <v>39.32</v>
+      </c>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B28" s="74" t="s">
-        <v>122</v>
+      <c r="B28" s="22" t="s">
+        <v>214</v>
       </c>
       <c r="C28" s="28">
-        <v>25.4</v>
+        <v>1.76</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="28">
-        <v>34.68</v>
-      </c>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="C29" s="26">
+        <v>0.13</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="22" t="s">
-        <v>120</v>
+      <c r="B30" s="71" t="s">
+        <v>123</v>
       </c>
       <c r="C30" s="28">
-        <v>39.32</v>
-      </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
+        <v>25.36</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="D31" s="23"/>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D32" s="23"/>
     </row>
@@ -4428,7 +4420,7 @@
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C39" s="7">
         <v>2.4300000000000002</v>
@@ -4437,7 +4429,7 @@
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C40" s="7">
         <v>2.4300000000000002</v>
@@ -4445,7 +4437,7 @@
     </row>
     <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C41" s="7">
         <v>3.71</v>
@@ -4453,7 +4445,7 @@
     </row>
     <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C42" s="7">
         <v>3</v>
@@ -4461,7 +4453,7 @@
     </row>
     <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C43" s="7">
         <v>1.92</v>
@@ -4469,12 +4461,12 @@
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C46" s="27">
         <v>0.2</v>
@@ -4482,7 +4474,7 @@
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C47" s="27">
         <v>0.42</v>
@@ -4490,7 +4482,7 @@
     </row>
     <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C48" s="27">
         <v>0.9</v>
@@ -4498,7 +4490,7 @@
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C49" s="27">
         <v>0.1</v>
@@ -4521,199 +4513,199 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="66" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="66" customWidth="1"/>
-    <col min="3" max="4" width="11.5" style="66"/>
-    <col min="5" max="5" width="17.5" style="66" customWidth="1"/>
-    <col min="6" max="16384" width="11.5" style="66"/>
+    <col min="1" max="1" width="33.6640625" style="63" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="63" customWidth="1"/>
+    <col min="3" max="4" width="11.5" style="63"/>
+    <col min="5" max="5" width="17.5" style="63" customWidth="1"/>
+    <col min="6" max="16384" width="11.5" style="63"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="71" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="71" t="s">
-        <v>208</v>
-      </c>
-      <c r="C1" s="71" t="s">
-        <v>207</v>
-      </c>
-      <c r="D1" s="71" t="s">
+      <c r="A1" s="68" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="71" t="s">
+      <c r="B1" s="68" t="s">
         <v>205</v>
       </c>
+      <c r="C1" s="68" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A2" s="70" t="s">
-        <v>204</v>
-      </c>
-      <c r="B2" s="69">
+      <c r="A2" s="67" t="s">
+        <v>201</v>
+      </c>
+      <c r="B2" s="66">
         <v>0.9</v>
       </c>
-      <c r="C2" s="68">
+      <c r="C2" s="65">
         <v>0.09</v>
       </c>
-      <c r="D2" s="66">
+      <c r="D2" s="63">
         <v>0.8</v>
       </c>
-      <c r="E2" s="66">
+      <c r="E2" s="63">
         <f t="shared" ref="E2:E10" si="0">C2*D2</f>
         <v>7.1999999999999995E-2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A3" s="70" t="s">
-        <v>203</v>
-      </c>
-      <c r="B3" s="69">
-        <v>1</v>
-      </c>
-      <c r="C3" s="68">
+      <c r="A3" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="66">
+        <v>1</v>
+      </c>
+      <c r="C3" s="65">
         <v>0.02</v>
       </c>
-      <c r="D3" s="66">
+      <c r="D3" s="63">
         <v>1.9</v>
       </c>
-      <c r="E3" s="66">
+      <c r="E3" s="63">
         <f t="shared" si="0"/>
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A4" s="70" t="s">
-        <v>202</v>
-      </c>
-      <c r="B4" s="69">
-        <v>1</v>
-      </c>
-      <c r="C4" s="68">
+      <c r="A4" s="67" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" s="66">
+        <v>1</v>
+      </c>
+      <c r="C4" s="65">
         <v>0.08</v>
       </c>
-      <c r="D4" s="66">
+      <c r="D4" s="63">
         <v>2</v>
       </c>
-      <c r="E4" s="66">
+      <c r="E4" s="63">
         <f t="shared" si="0"/>
         <v>0.16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A5" s="70" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" s="69">
-        <v>1</v>
-      </c>
-      <c r="C5" s="68">
+      <c r="A5" s="67" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" s="66">
+        <v>1</v>
+      </c>
+      <c r="C5" s="65">
         <v>0.18</v>
       </c>
-      <c r="D5" s="66">
+      <c r="D5" s="63">
         <v>0.7</v>
       </c>
-      <c r="E5" s="66">
+      <c r="E5" s="63">
         <f t="shared" si="0"/>
         <v>0.126</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A6" s="70" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="69">
-        <v>1</v>
-      </c>
-      <c r="C6" s="68">
+      <c r="A6" s="67" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="66">
+        <v>1</v>
+      </c>
+      <c r="C6" s="65">
         <v>0.02</v>
       </c>
-      <c r="D6" s="66">
+      <c r="D6" s="63">
         <v>0.7</v>
       </c>
-      <c r="E6" s="66">
+      <c r="E6" s="63">
         <f t="shared" si="0"/>
         <v>1.3999999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A7" s="70" t="s">
-        <v>199</v>
-      </c>
-      <c r="B7" s="69">
+      <c r="A7" s="67" t="s">
+        <v>196</v>
+      </c>
+      <c r="B7" s="66">
         <v>0.93</v>
       </c>
-      <c r="C7" s="68">
+      <c r="C7" s="65">
         <v>0.45</v>
       </c>
-      <c r="D7" s="66">
+      <c r="D7" s="63">
         <v>0.9</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="63">
         <f t="shared" si="0"/>
         <v>0.40500000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A8" s="70" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="69">
+      <c r="A8" s="67" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" s="66">
         <v>0.5</v>
       </c>
-      <c r="C8" s="68">
+      <c r="C8" s="65">
         <v>0.03</v>
       </c>
-      <c r="D8" s="66">
-        <v>0</v>
-      </c>
-      <c r="E8" s="66">
+      <c r="D8" s="63">
+        <v>0</v>
+      </c>
+      <c r="E8" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A9" s="70" t="s">
-        <v>197</v>
-      </c>
-      <c r="B9" s="69">
+      <c r="A9" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="B9" s="66">
         <v>0.5</v>
       </c>
-      <c r="C9" s="68">
+      <c r="C9" s="65">
         <v>0.11</v>
       </c>
-      <c r="D9" s="66">
-        <v>0</v>
-      </c>
-      <c r="E9" s="66">
+      <c r="D9" s="63">
+        <v>0</v>
+      </c>
+      <c r="E9" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A10" s="70" t="s">
-        <v>196</v>
-      </c>
-      <c r="B10" s="69">
+      <c r="A10" s="67" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10" s="66">
         <v>0.98</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="65">
         <v>0.01</v>
       </c>
-      <c r="D10" s="66">
+      <c r="D10" s="63">
         <v>0.6</v>
       </c>
-      <c r="E10" s="66">
+      <c r="E10" s="63">
         <f t="shared" si="0"/>
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="C11" s="67"/>
+      <c r="C11" s="64"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4729,7 +4721,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -4741,7 +4733,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="34" t="s">
         <v>1</v>
@@ -5376,7 +5368,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5393,10 +5385,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="34" t="s">
         <v>144</v>
-      </c>
-      <c r="C1" s="34" t="s">
-        <v>145</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>50</v>
@@ -5411,16 +5403,16 @@
         <v>53</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="I1" s="59" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>145</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="K1" s="59" t="s">
         <v>168</v>
+      </c>
+      <c r="K1" s="57" t="s">
+        <v>167</v>
       </c>
       <c r="L1" s="34" t="s">
         <v>37</v>
@@ -5451,7 +5443,7 @@
       <c r="H2" s="32">
         <v>173766200</v>
       </c>
-      <c r="I2" s="60">
+      <c r="I2" s="33">
         <f t="shared" ref="I2:I15" si="0">D2+E2+F2+G2</f>
         <v>44709100</v>
       </c>
@@ -5459,7 +5451,7 @@
         <f t="shared" ref="J2:J15" si="1">(B2 + stillbirth*B2/(1000-stillbirth))/(1-abortion)</f>
         <v>3650590.4685349194</v>
       </c>
-      <c r="K2" s="61">
+      <c r="K2" s="58">
         <f t="shared" ref="K2:K15" si="2">D2/I2</f>
         <v>0.19650809343064388</v>
       </c>
@@ -5493,7 +5485,7 @@
       <c r="H3" s="32">
         <v>175848400</v>
       </c>
-      <c r="I3" s="60">
+      <c r="I3" s="33">
         <f t="shared" si="0"/>
         <v>45692200</v>
       </c>
@@ -5501,7 +5493,7 @@
         <f t="shared" si="1"/>
         <v>3622037.632993402</v>
       </c>
-      <c r="K3" s="61">
+      <c r="K3" s="58">
         <f t="shared" si="2"/>
         <v>0.19560012431005733</v>
       </c>
@@ -5535,7 +5527,7 @@
       <c r="H4" s="32">
         <v>177930600</v>
       </c>
-      <c r="I4" s="60">
+      <c r="I4" s="33">
         <f t="shared" si="0"/>
         <v>46675300</v>
       </c>
@@ -5543,7 +5535,7 @@
         <f t="shared" si="1"/>
         <v>3591353.7424015561</v>
       </c>
-      <c r="K4" s="61">
+      <c r="K4" s="58">
         <f t="shared" si="2"/>
         <v>0.19473040344679096</v>
       </c>
@@ -5577,7 +5569,7 @@
       <c r="H5" s="32">
         <v>180012800</v>
       </c>
-      <c r="I5" s="60">
+      <c r="I5" s="33">
         <f t="shared" si="0"/>
         <v>47658400.000000015</v>
       </c>
@@ -5585,7 +5577,7 @@
         <f t="shared" si="1"/>
         <v>3558361.8967828737</v>
       </c>
-      <c r="K5" s="61">
+      <c r="K5" s="58">
         <f t="shared" si="2"/>
         <v>0.19389656387960991</v>
       </c>
@@ -5619,7 +5611,7 @@
       <c r="H6" s="32">
         <v>182095000</v>
       </c>
-      <c r="I6" s="60">
+      <c r="I6" s="33">
         <f t="shared" si="0"/>
         <v>48641500.000000015</v>
       </c>
@@ -5627,7 +5619,7 @@
         <f t="shared" si="1"/>
         <v>3527004.6069471212</v>
       </c>
-      <c r="K6" s="61">
+      <c r="K6" s="58">
         <f t="shared" si="2"/>
         <v>0.1930964300031866</v>
       </c>
@@ -5661,7 +5653,7 @@
       <c r="H7" s="32">
         <v>183822800</v>
       </c>
-      <c r="I7" s="60">
+      <c r="I7" s="33">
         <f t="shared" si="0"/>
         <v>49111300.000000015</v>
       </c>
@@ -5669,7 +5661,7 @@
         <f t="shared" si="1"/>
         <v>3493354.6934158299</v>
       </c>
-      <c r="K7" s="61">
+      <c r="K7" s="58">
         <f t="shared" si="2"/>
         <v>0.1833447699409301</v>
       </c>
@@ -5703,7 +5695,7 @@
       <c r="H8" s="32">
         <v>185550600</v>
       </c>
-      <c r="I8" s="60">
+      <c r="I8" s="33">
         <f t="shared" si="0"/>
         <v>49581100.000000007</v>
       </c>
@@ -5711,7 +5703,7 @@
         <f t="shared" si="1"/>
         <v>3457383.8521927581</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="58">
         <f t="shared" si="2"/>
         <v>0.17377791134121673</v>
       </c>
@@ -5745,7 +5737,7 @@
       <c r="H9" s="32">
         <v>187278400</v>
       </c>
-      <c r="I9" s="60">
+      <c r="I9" s="33">
         <f t="shared" si="0"/>
         <v>50050900.000000007</v>
       </c>
@@ -5753,7 +5745,7 @@
         <f t="shared" si="1"/>
         <v>3419187.609265219</v>
       </c>
-      <c r="K9" s="61">
+      <c r="K9" s="58">
         <f t="shared" si="2"/>
         <v>0.16439065031797631</v>
       </c>
@@ -5787,7 +5779,7 @@
       <c r="H10" s="32">
         <v>189006200</v>
       </c>
-      <c r="I10" s="60">
+      <c r="I10" s="33">
         <f t="shared" si="0"/>
         <v>50520700.000000007</v>
       </c>
@@ -5795,7 +5787,7 @@
         <f t="shared" si="1"/>
         <v>3378798.9859621613</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="58">
         <f t="shared" si="2"/>
         <v>0.15517797655218554</v>
       </c>
@@ -5829,7 +5821,7 @@
       <c r="H11" s="32">
         <v>190734000</v>
       </c>
-      <c r="I11" s="60">
+      <c r="I11" s="33">
         <f t="shared" si="0"/>
         <v>50990500</v>
       </c>
@@ -5837,7 +5829,7 @@
         <f t="shared" si="1"/>
         <v>3344756.3544830228</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="58">
         <f t="shared" si="2"/>
         <v>0.1461350643747365</v>
       </c>
@@ -5871,7 +5863,7 @@
       <c r="H12" s="32">
         <v>192287600</v>
       </c>
-      <c r="I12" s="60">
+      <c r="I12" s="33">
         <f t="shared" si="0"/>
         <v>51333400</v>
       </c>
@@ -5879,7 +5871,7 @@
         <f t="shared" si="1"/>
         <v>3308667.5799422786</v>
       </c>
-      <c r="K12" s="61">
+      <c r="K12" s="58">
         <f t="shared" si="2"/>
         <v>0.14438357872262508</v>
       </c>
@@ -5913,7 +5905,7 @@
       <c r="H13" s="32">
         <v>193841200</v>
       </c>
-      <c r="I13" s="60">
+      <c r="I13" s="33">
         <f t="shared" si="0"/>
         <v>51676300</v>
       </c>
@@ -5921,7 +5913,7 @@
         <f t="shared" si="1"/>
         <v>3270569.2216684073</v>
       </c>
-      <c r="K13" s="61">
+      <c r="K13" s="58">
         <f t="shared" si="2"/>
         <v>0.14265533716616713</v>
       </c>
@@ -5955,7 +5947,7 @@
       <c r="H14" s="32">
         <v>195394800</v>
       </c>
-      <c r="I14" s="60">
+      <c r="I14" s="33">
         <f t="shared" si="0"/>
         <v>52019200</v>
       </c>
@@ -5963,7 +5955,7 @@
         <f t="shared" si="1"/>
         <v>3230515.5289875376</v>
       </c>
-      <c r="K14" s="61">
+      <c r="K14" s="58">
         <f t="shared" si="2"/>
         <v>0.14094988004429135</v>
       </c>
@@ -5997,7 +5989,7 @@
       <c r="H15" s="32">
         <v>196948400</v>
       </c>
-      <c r="I15" s="60">
+      <c r="I15" s="33">
         <f t="shared" si="0"/>
         <v>52362100</v>
       </c>
@@ -6005,7 +5997,7 @@
         <f t="shared" si="1"/>
         <v>3188527.7298968509</v>
       </c>
-      <c r="K15" s="61">
+      <c r="K15" s="58">
         <f t="shared" si="2"/>
         <v>0.139266759736527</v>
       </c>
@@ -6039,7 +6031,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="41" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -6062,10 +6054,10 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="52">
         <f>1-SUM(C3:C5)</f>
@@ -6091,7 +6083,7 @@
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5"/>
       <c r="B3" s="16" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="42">
         <v>0.22600000000000001</v>
@@ -6112,7 +6104,7 @@
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="42">
         <v>0.10199999999999999</v>
@@ -6133,7 +6125,7 @@
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C5" s="42">
         <v>3.7999999999999999E-2</v>
@@ -6169,10 +6161,10 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C8" s="52">
         <f t="shared" ref="C8:G8" si="1">1-SUM(C9:C11)</f>
@@ -6197,7 +6189,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="42">
         <v>0.23300000000000001</v>
@@ -6217,7 +6209,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" s="42">
         <v>0.15</v>
@@ -6237,7 +6229,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C11" s="42">
         <v>4.9000000000000002E-2</v>
@@ -6315,7 +6307,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C14" s="53">
         <v>0.1</v>
@@ -6454,7 +6446,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="41" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
@@ -6479,8 +6471,8 @@
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="75" t="s">
-        <v>212</v>
+      <c r="B2" s="72" t="s">
+        <v>209</v>
       </c>
       <c r="C2" s="42">
         <v>0.80299999999999994</v>
@@ -6499,8 +6491,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B3" s="75" t="s">
-        <v>213</v>
+      <c r="B3" s="72" t="s">
+        <v>210</v>
       </c>
       <c r="C3" s="42">
         <v>6.8000000000000005E-2</v>
@@ -6519,8 +6511,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B4" s="75" t="s">
-        <v>214</v>
+      <c r="B4" s="72" t="s">
+        <v>211</v>
       </c>
       <c r="C4" s="42">
         <v>0.107</v>
@@ -6539,8 +6531,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="B5" s="75" t="s">
-        <v>215</v>
+      <c r="B5" s="72" t="s">
+        <v>212</v>
       </c>
       <c r="C5" s="52">
         <f>1-SUM(C2:C4)</f>
@@ -6576,7 +6568,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6587,10 +6579,10 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1">
         <v>2010</v>
@@ -6622,10 +6614,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="42"/>
@@ -6642,10 +6634,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -6662,10 +6654,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -6679,7 +6671,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B7" s="20" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
@@ -6693,7 +6685,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B8" s="20" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
@@ -6705,15 +6697,12 @@
       <c r="J8" s="42"/>
       <c r="K8" s="42"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B9" s="20"/>
-    </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
@@ -6727,7 +6716,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="B11" s="56" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="42"/>
@@ -6741,10 +6730,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="B13" s="22" t="s">
-        <v>192</v>
+        <v>93</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>191</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
@@ -6757,8 +6746,8 @@
       <c r="K13" s="42"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="B14" s="56" t="s">
-        <v>193</v>
+      <c r="B14" s="22" t="s">
+        <v>213</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
@@ -6797,18 +6786,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="47" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="45" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>210</v>
+        <v>160</v>
+      </c>
+      <c r="B1" s="70" t="s">
+        <v>207</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B2" s="44" t="s">
         <v>94</v>
@@ -6883,7 +6872,7 @@
     </row>
     <row r="11" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="50">
         <f>SUM(C2:C10)</f>
@@ -6931,7 +6920,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B17" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="50">
         <f>SUM(C13:C16)</f>
@@ -7067,7 +7056,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7230,11 +7219,11 @@
       <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="62">
+      <c r="E4" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="F4" s="62">
+      <c r="F4" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
@@ -7268,7 +7257,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -7276,11 +7265,11 @@
       <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="62">
+      <c r="E5" s="59">
         <f>food_insecure*(1-frac_malaria_risk)</f>
         <v>0.32400000000000001</v>
       </c>
-      <c r="F5" s="62">
+      <c r="F5" s="59">
         <f>food_insecure*(1-frac_malaria_risk)</f>
         <v>0.32400000000000001</v>
       </c>
@@ -7314,7 +7303,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -7322,11 +7311,11 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="62">
+      <c r="E6" s="59">
         <f>food_insecure*frac_malaria_risk</f>
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="F6" s="62">
+      <c r="F6" s="59">
         <f>food_insecure*frac_malaria_risk</f>
         <v>3.5999999999999997E-2</v>
       </c>
@@ -7360,7 +7349,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -7368,15 +7357,15 @@
       <c r="D7" s="2">
         <v>0</v>
       </c>
-      <c r="E7" s="62">
+      <c r="E7" s="59">
         <f>(1-frac_malaria_risk)</f>
         <v>0.9</v>
       </c>
-      <c r="F7" s="62">
+      <c r="F7" s="59">
         <f>(1-frac_malaria_risk)</f>
         <v>0.9</v>
       </c>
-      <c r="G7" s="62">
+      <c r="G7" s="59">
         <f>(1-frac_malaria_risk)</f>
         <v>0.9</v>
       </c>
@@ -7407,7 +7396,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="16" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -7415,15 +7404,15 @@
       <c r="D8" s="2">
         <v>0</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="F8" s="62">
+      <c r="F8" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="G8" s="62">
+      <c r="G8" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
@@ -7459,19 +7448,19 @@
       <c r="C9" s="17">
         <v>0</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="E9" s="62">
+      <c r="E9" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="F9" s="62">
+      <c r="F9" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="G9" s="62">
+      <c r="G9" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
@@ -7590,9 +7579,9 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="65">
+        <v>192</v>
+      </c>
+      <c r="C12" s="62">
         <v>1</v>
       </c>
       <c r="D12" s="17">
@@ -7657,19 +7646,19 @@
       <c r="G14" s="2">
         <v>0</v>
       </c>
-      <c r="H14" s="62">
+      <c r="H14" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="I14" s="62">
+      <c r="I14" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="J14" s="62">
+      <c r="J14" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
-      <c r="K14" s="62">
+      <c r="K14" s="59">
         <f>food_insecure</f>
         <v>0.36</v>
       </c>
@@ -7706,19 +7695,19 @@
       <c r="G15" s="2">
         <v>0</v>
       </c>
-      <c r="H15" s="63">
+      <c r="H15" s="60">
         <f>1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
-      <c r="I15" s="63">
+      <c r="I15" s="60">
         <f>1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
-      <c r="J15" s="63">
+      <c r="J15" s="60">
         <f>1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
-      <c r="K15" s="63">
+      <c r="K15" s="60">
         <f>1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
@@ -7754,19 +7743,19 @@
       <c r="G16" s="2">
         <v>0</v>
       </c>
-      <c r="H16" s="62">
+      <c r="H16" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="I16" s="62">
+      <c r="I16" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="J16" s="62">
+      <c r="J16" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="K16" s="62">
+      <c r="K16" s="59">
         <f>frac_malaria_risk</f>
         <v>0.1</v>
       </c>
@@ -7802,19 +7791,19 @@
       <c r="G17" s="2">
         <v>0</v>
       </c>
-      <c r="H17" s="63">
+      <c r="H17" s="60">
         <f xml:space="preserve"> 1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
-      <c r="I17" s="63">
+      <c r="I17" s="60">
         <f xml:space="preserve"> 1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
-      <c r="J17" s="63">
+      <c r="J17" s="60">
         <f xml:space="preserve"> 1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
-      <c r="K17" s="63">
+      <c r="K17" s="60">
         <f xml:space="preserve"> 1-frac_malaria_risk</f>
         <v>0.9</v>
       </c>
@@ -7850,19 +7839,19 @@
       <c r="G18" s="2">
         <v>0</v>
       </c>
-      <c r="H18" s="63">
+      <c r="H18" s="60">
         <f t="shared" ref="H18:K19" si="0">frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="I18" s="63">
+      <c r="I18" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="J18" s="63">
+      <c r="J18" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="K18" s="63">
+      <c r="K18" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -7898,19 +7887,19 @@
       <c r="G19" s="2">
         <v>0</v>
       </c>
-      <c r="H19" s="63">
+      <c r="H19" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="I19" s="63">
+      <c r="I19" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="J19" s="63">
+      <c r="J19" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="K19" s="63">
+      <c r="K19" s="60">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
@@ -7964,17 +7953,17 @@
       <c r="K21" s="11">
         <v>0</v>
       </c>
-      <c r="L21" s="62">
+      <c r="L21" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*1*school_attendance</f>
         <v>0.114048</v>
       </c>
-      <c r="M21" s="62">
-        <v>0</v>
-      </c>
-      <c r="N21" s="62">
-        <v>0</v>
-      </c>
-      <c r="O21" s="62">
+      <c r="M21" s="59">
+        <v>0</v>
+      </c>
+      <c r="N21" s="59">
+        <v>0</v>
+      </c>
+      <c r="O21" s="59">
         <v>0</v>
       </c>
     </row>
@@ -8009,19 +7998,19 @@
       <c r="K22" s="11">
         <v>0</v>
       </c>
-      <c r="L22" s="62">
+      <c r="L22" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.7)*(1-school_attendance)</f>
         <v>0.1469664</v>
       </c>
-      <c r="M22" s="62">
+      <c r="M22" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.7)</f>
         <v>0.2268</v>
       </c>
-      <c r="N22" s="62">
+      <c r="N22" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.7)</f>
         <v>0.2268</v>
       </c>
-      <c r="O22" s="62">
+      <c r="O22" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.7)</f>
         <v>0.2268</v>
       </c>
@@ -8057,19 +8046,19 @@
       <c r="K23" s="11">
         <v>0</v>
       </c>
-      <c r="L23" s="62">
+      <c r="L23" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)*(1-school_attendance)</f>
         <v>6.2985600000000003E-2</v>
       </c>
-      <c r="M23" s="62">
+      <c r="M23" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)</f>
         <v>9.7199999999999995E-2</v>
       </c>
-      <c r="N23" s="62">
+      <c r="N23" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)</f>
         <v>9.7199999999999995E-2</v>
       </c>
-      <c r="O23" s="62">
+      <c r="O23" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)</f>
         <v>9.7199999999999995E-2</v>
       </c>
@@ -8105,17 +8094,17 @@
       <c r="K24" s="11">
         <v>0</v>
       </c>
-      <c r="L24" s="62">
+      <c r="L24" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*1*school_attendance</f>
         <v>0.20275200000000002</v>
       </c>
-      <c r="M24" s="62">
-        <v>0</v>
-      </c>
-      <c r="N24" s="62">
-        <v>0</v>
-      </c>
-      <c r="O24" s="62">
+      <c r="M24" s="59">
+        <v>0</v>
+      </c>
+      <c r="N24" s="59">
+        <v>0</v>
+      </c>
+      <c r="O24" s="59">
         <v>0</v>
       </c>
     </row>
@@ -8150,19 +8139,19 @@
       <c r="K25" s="11">
         <v>0</v>
       </c>
-      <c r="L25" s="62">
+      <c r="L25" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.49)*(1-school_attendance)</f>
         <v>0.18289152000000003</v>
       </c>
-      <c r="M25" s="62">
+      <c r="M25" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.49)</f>
         <v>0.28224000000000005</v>
       </c>
-      <c r="N25" s="62">
+      <c r="N25" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.49)</f>
         <v>0.28224000000000005</v>
       </c>
-      <c r="O25" s="62">
+      <c r="O25" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.49)</f>
         <v>0.28224000000000005</v>
       </c>
@@ -8198,19 +8187,19 @@
       <c r="K26" s="11">
         <v>0</v>
       </c>
-      <c r="L26" s="62">
+      <c r="L26" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.21)*(1-school_attendance)</f>
         <v>7.8382080000000007E-2</v>
       </c>
-      <c r="M26" s="62">
+      <c r="M26" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.21)</f>
         <v>0.12096000000000001</v>
       </c>
-      <c r="N26" s="62">
+      <c r="N26" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.21)</f>
         <v>0.12096000000000001</v>
       </c>
-      <c r="O26" s="62">
+      <c r="O26" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.21)</f>
         <v>0.12096000000000001</v>
       </c>
@@ -8246,19 +8235,19 @@
       <c r="K27" s="11">
         <v>0</v>
       </c>
-      <c r="L27" s="62">
+      <c r="L27" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.3)*(1-school_attendance)</f>
         <v>0.11197440000000002</v>
       </c>
-      <c r="M27" s="62">
+      <c r="M27" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.3)</f>
         <v>0.17280000000000001</v>
       </c>
-      <c r="N27" s="62">
+      <c r="N27" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.3)</f>
         <v>0.17280000000000001</v>
       </c>
-      <c r="O27" s="62">
+      <c r="O27" s="59">
         <f>(1-food_insecure)*(1-frac_malaria_risk)*(0.3)</f>
         <v>0.17280000000000001</v>
       </c>
@@ -8295,17 +8284,17 @@
       <c r="K28" s="11">
         <v>0</v>
       </c>
-      <c r="L28" s="62">
+      <c r="L28" s="59">
         <f>food_insecure*(frac_malaria_risk)*1*school_attendance</f>
         <v>1.2671999999999998E-2</v>
       </c>
-      <c r="M28" s="62">
-        <v>0</v>
-      </c>
-      <c r="N28" s="62">
-        <v>0</v>
-      </c>
-      <c r="O28" s="62">
+      <c r="M28" s="59">
+        <v>0</v>
+      </c>
+      <c r="N28" s="59">
+        <v>0</v>
+      </c>
+      <c r="O28" s="59">
         <v>0</v>
       </c>
     </row>
@@ -8340,19 +8329,19 @@
       <c r="K29" s="11">
         <v>0</v>
       </c>
-      <c r="L29" s="62">
+      <c r="L29" s="59">
         <f>food_insecure*(frac_malaria_risk)*(0.7)*(1-school_attendance)</f>
         <v>1.63296E-2</v>
       </c>
-      <c r="M29" s="62">
+      <c r="M29" s="59">
         <f>food_insecure*(frac_malaria_risk)*(0.7)</f>
         <v>2.5199999999999997E-2</v>
       </c>
-      <c r="N29" s="62">
+      <c r="N29" s="59">
         <f>food_insecure*(frac_malaria_risk)*(0.7)</f>
         <v>2.5199999999999997E-2</v>
       </c>
-      <c r="O29" s="62">
+      <c r="O29" s="59">
         <f>food_insecure*(frac_malaria_risk)*(0.7)</f>
         <v>2.5199999999999997E-2</v>
       </c>
@@ -8388,19 +8377,19 @@
       <c r="K30" s="11">
         <v>0</v>
       </c>
-      <c r="L30" s="62">
+      <c r="L30" s="59">
         <f>food_insecure*(frac_malaria_risk)*(0.3)*(1-school_attendance)</f>
         <v>6.9983999999999992E-3</v>
       </c>
-      <c r="M30" s="62">
+      <c r="M30" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)</f>
         <v>9.7199999999999995E-2</v>
       </c>
-      <c r="N30" s="62">
+      <c r="N30" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)</f>
         <v>9.7199999999999995E-2</v>
       </c>
-      <c r="O30" s="62">
+      <c r="O30" s="59">
         <f>food_insecure*(1-frac_malaria_risk)*(0.3)</f>
         <v>9.7199999999999995E-2</v>
       </c>
@@ -8436,17 +8425,17 @@
       <c r="K31" s="11">
         <v>0</v>
       </c>
-      <c r="L31" s="62">
+      <c r="L31" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*1*school_attendance</f>
         <v>2.2527999999999999E-2</v>
       </c>
-      <c r="M31" s="62">
-        <v>0</v>
-      </c>
-      <c r="N31" s="62">
-        <v>0</v>
-      </c>
-      <c r="O31" s="62">
+      <c r="M31" s="59">
+        <v>0</v>
+      </c>
+      <c r="N31" s="59">
+        <v>0</v>
+      </c>
+      <c r="O31" s="59">
         <v>0</v>
       </c>
     </row>
@@ -8481,19 +8470,19 @@
       <c r="K32" s="11">
         <v>0</v>
       </c>
-      <c r="L32" s="62">
+      <c r="L32" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.49)*(1-school_attendance)</f>
         <v>2.0321280000000001E-2</v>
       </c>
-      <c r="M32" s="62">
+      <c r="M32" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.49)</f>
         <v>3.1359999999999999E-2</v>
       </c>
-      <c r="N32" s="62">
+      <c r="N32" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.49)</f>
         <v>3.1359999999999999E-2</v>
       </c>
-      <c r="O32" s="62">
+      <c r="O32" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.49)</f>
         <v>3.1359999999999999E-2</v>
       </c>
@@ -8529,19 +8518,19 @@
       <c r="K33" s="11">
         <v>0</v>
       </c>
-      <c r="L33" s="62">
+      <c r="L33" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.21)*(1-school_attendance)</f>
         <v>8.7091200000000007E-3</v>
       </c>
-      <c r="M33" s="62">
+      <c r="M33" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.21)</f>
         <v>1.3440000000000001E-2</v>
       </c>
-      <c r="N33" s="62">
+      <c r="N33" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.21)</f>
         <v>1.3440000000000001E-2</v>
       </c>
-      <c r="O33" s="62">
+      <c r="O33" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.21)</f>
         <v>1.3440000000000001E-2</v>
       </c>
@@ -8577,19 +8566,19 @@
       <c r="K34" s="11">
         <v>0</v>
       </c>
-      <c r="L34" s="62">
+      <c r="L34" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.3)*(1-school_attendance)</f>
         <v>1.2441599999999999E-2</v>
       </c>
-      <c r="M34" s="62">
+      <c r="M34" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.3)</f>
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="N34" s="62">
+      <c r="N34" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.3)</f>
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="O34" s="62">
+      <c r="O34" s="59">
         <f>(1-food_insecure)*(frac_malaria_risk)*(0.3)</f>
         <v>1.9199999999999998E-2</v>
       </c>
@@ -8625,16 +8614,16 @@
       <c r="K35" s="11">
         <v>0</v>
       </c>
-      <c r="L35" s="62">
-        <v>1</v>
-      </c>
-      <c r="M35" s="62">
-        <v>1</v>
-      </c>
-      <c r="N35" s="62">
-        <v>1</v>
-      </c>
-      <c r="O35" s="62">
+      <c r="L35" s="59">
+        <v>1</v>
+      </c>
+      <c r="M35" s="59">
+        <v>1</v>
+      </c>
+      <c r="N35" s="59">
+        <v>1</v>
+      </c>
+      <c r="O35" s="59">
         <v>1</v>
       </c>
     </row>
@@ -8669,16 +8658,16 @@
       <c r="K36" s="11">
         <v>0</v>
       </c>
-      <c r="L36" s="64">
-        <v>1</v>
-      </c>
-      <c r="M36" s="64">
-        <v>1</v>
-      </c>
-      <c r="N36" s="64">
-        <v>1</v>
-      </c>
-      <c r="O36" s="64">
+      <c r="L36" s="61">
+        <v>1</v>
+      </c>
+      <c r="M36" s="61">
+        <v>1</v>
+      </c>
+      <c r="N36" s="61">
+        <v>1</v>
+      </c>
+      <c r="O36" s="61">
         <v>1</v>
       </c>
     </row>
@@ -9140,55 +9129,55 @@
       <c r="B48" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="63">
+      <c r="C48" s="60">
         <f t="shared" ref="C48:O48" si="1">frac_malaria_risk</f>
         <v>0.1</v>
       </c>
-      <c r="D48" s="63">
+      <c r="D48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="E48" s="63">
+      <c r="E48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="F48" s="63">
+      <c r="F48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="G48" s="63">
+      <c r="G48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="H48" s="63">
+      <c r="H48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="I48" s="63">
+      <c r="I48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="J48" s="63">
+      <c r="J48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="K48" s="63">
+      <c r="K48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="L48" s="63">
+      <c r="L48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="M48" s="63">
+      <c r="M48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="N48" s="63">
+      <c r="N48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
-      <c r="O48" s="63">
+      <c r="O48" s="60">
         <f t="shared" si="1"/>
         <v>0.1</v>
       </c>
@@ -9203,47 +9192,47 @@
       <c r="D49" s="17">
         <v>0</v>
       </c>
-      <c r="E49" s="63">
+      <c r="E49" s="60">
         <f t="shared" ref="E49:O49" si="2">frac_wheat</f>
         <v>0.12</v>
       </c>
-      <c r="F49" s="63">
+      <c r="F49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="G49" s="63">
+      <c r="G49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="H49" s="63">
+      <c r="H49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="I49" s="63">
+      <c r="I49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="J49" s="63">
+      <c r="J49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="K49" s="63">
+      <c r="K49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="L49" s="63">
+      <c r="L49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="M49" s="63">
+      <c r="M49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="N49" s="63">
+      <c r="N49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
-      <c r="O49" s="63">
+      <c r="O49" s="60">
         <f t="shared" si="2"/>
         <v>0.12</v>
       </c>
@@ -9258,47 +9247,47 @@
       <c r="D50" s="17">
         <v>0</v>
       </c>
-      <c r="E50" s="63">
+      <c r="E50" s="60">
         <f t="shared" ref="E50:O50" si="3">frac_maize</f>
         <v>0.05</v>
       </c>
-      <c r="F50" s="63">
+      <c r="F50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="G50" s="63">
+      <c r="G50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="H50" s="63">
+      <c r="H50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="I50" s="63">
+      <c r="I50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="J50" s="63">
+      <c r="J50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="K50" s="63">
+      <c r="K50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="L50" s="63">
+      <c r="L50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="M50" s="63">
+      <c r="M50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="N50" s="63">
+      <c r="N50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="O50" s="63">
+      <c r="O50" s="60">
         <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
@@ -9313,47 +9302,47 @@
       <c r="D51" s="17">
         <v>0</v>
       </c>
-      <c r="E51" s="63">
+      <c r="E51" s="60">
         <f t="shared" ref="E51:O51" si="4">frac_rice</f>
         <v>0.8</v>
       </c>
-      <c r="F51" s="63">
+      <c r="F51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="G51" s="63">
+      <c r="G51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="H51" s="63">
+      <c r="H51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="I51" s="63">
+      <c r="I51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="J51" s="63">
+      <c r="J51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="K51" s="63">
+      <c r="K51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="L51" s="63">
+      <c r="L51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="M51" s="63">
+      <c r="M51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="N51" s="63">
+      <c r="N51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="O51" s="63">
+      <c r="O51" s="60">
         <f t="shared" si="4"/>
         <v>0.8</v>
       </c>

</xml_diff>

<commit_message>
A couple fixes, script for plotting with hardcoded example
</commit_message>
<xml_diff>
--- a/applications/master/data/national/master_input.xlsx
+++ b/applications/master/data/national/master_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/Github Projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{50A48E2E-96A0-C347-8378-5EDD1535F14F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{36EAB655-899C-6B4E-962F-BE91711EA83D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4840" yWindow="-20400" windowWidth="25600" windowHeight="15540" tabRatio="961" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -4130,8 +4130,8 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6019,8 +6019,8 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6060,24 +6060,24 @@
         <v>151</v>
       </c>
       <c r="C2" s="52">
-        <f>1-SUM(C3:C5)</f>
-        <v>0.63400000000000001</v>
+        <f>1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE)</f>
+        <v>0.53200836191885958</v>
       </c>
       <c r="D2" s="52">
-        <f t="shared" ref="D2:G2" si="0">1-SUM(D3:D5)</f>
-        <v>0.63400000000000001</v>
+        <f t="shared" ref="D2:G2" si="0">1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE)</f>
+        <v>0.53200836191885958</v>
       </c>
       <c r="E2" s="52">
         <f t="shared" si="0"/>
-        <v>0.49</v>
+        <v>0.44274864978114037</v>
       </c>
       <c r="F2" s="52">
         <f t="shared" si="0"/>
-        <v>0.28000000000000003</v>
+        <v>0.24285617786005109</v>
       </c>
       <c r="G2" s="52">
         <f t="shared" si="0"/>
-        <v>0.25349999999999995</v>
+        <v>0.2168920625348294</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6085,20 +6085,25 @@
       <c r="B3" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="C3" s="42">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="D3" s="42">
-        <v>0.22600000000000001</v>
-      </c>
-      <c r="E3" s="42">
-        <v>0.314</v>
-      </c>
-      <c r="F3" s="42">
-        <v>0.33899999999999997</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0.33250000000000002</v>
+      <c r="C3" s="52">
+        <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C4:C5), 0, 1) + 1, 0, 1, TRUE) - SUM(C4:C5)</f>
+        <v>0.3279916380811404</v>
+      </c>
+      <c r="D3" s="52">
+        <f t="shared" ref="D3:G3" si="1">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D4:D5), 0, 1) + 1, 0, 1, TRUE) - SUM(D4:D5)</f>
+        <v>0.3279916380811404</v>
+      </c>
+      <c r="E3" s="52">
+        <f t="shared" si="1"/>
+        <v>0.36125135021885962</v>
+      </c>
+      <c r="F3" s="52">
+        <f t="shared" si="1"/>
+        <v>0.3761438221399489</v>
+      </c>
+      <c r="G3" s="52">
+        <f t="shared" si="1"/>
+        <v>0.36910793746517057</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6167,44 +6172,49 @@
         <v>154</v>
       </c>
       <c r="C8" s="52">
-        <f t="shared" ref="C8:G8" si="1">1-SUM(C9:C11)</f>
-        <v>0.56800000000000006</v>
+        <f>1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE)</f>
+        <v>0.43848891822683433</v>
       </c>
       <c r="D8" s="52">
-        <f t="shared" si="1"/>
-        <v>0.56800000000000006</v>
+        <f t="shared" ref="D8:G8" si="2">1-_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE)</f>
+        <v>0.43848891822683433</v>
       </c>
       <c r="E8" s="52">
-        <f t="shared" si="1"/>
-        <v>0.58650000000000002</v>
+        <f t="shared" si="2"/>
+        <v>0.46325746477389407</v>
       </c>
       <c r="F8" s="52">
-        <f t="shared" si="1"/>
-        <v>0.54900000000000004</v>
+        <f t="shared" si="2"/>
+        <v>0.51282536329943151</v>
       </c>
       <c r="G8" s="52">
-        <f t="shared" si="1"/>
-        <v>0.49</v>
+        <f t="shared" si="2"/>
+        <v>0.55784394006702964</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="C9" s="42">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="D9" s="42">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="E9" s="42">
-        <v>0.23149999999999998</v>
-      </c>
-      <c r="F9" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="G9" s="42">
-        <v>0.38400000000000001</v>
+      <c r="C9" s="52">
+        <f>_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(C10:C11), 0, 1) + 1, 0, 1, TRUE) - SUM(C10:C11)</f>
+        <v>0.36251108177316566</v>
+      </c>
+      <c r="D9" s="52">
+        <f t="shared" ref="D9:G9" si="3">_xlfn.NORM.DIST(_xlfn.NORM.INV(SUM(D10:D11), 0, 1) + 1, 0, 1, TRUE) - SUM(D10:D11)</f>
+        <v>0.36251108177316566</v>
+      </c>
+      <c r="E9" s="52">
+        <f t="shared" si="3"/>
+        <v>0.35474253522610594</v>
+      </c>
+      <c r="F9" s="52">
+        <f t="shared" si="3"/>
+        <v>0.33617463670056846</v>
+      </c>
+      <c r="G9" s="52">
+        <f t="shared" si="3"/>
+        <v>0.31615605993297041</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6354,55 +6364,55 @@
         <v>87</v>
       </c>
       <c r="C15" s="52">
-        <f t="shared" ref="C15:O15" si="2">iron_deficiency_anaemia*C14</f>
+        <f t="shared" ref="C15:O15" si="4">iron_deficiency_anaemia*C14</f>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="D15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="E15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.31079999999999997</v>
       </c>
       <c r="F15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.23100000000000001</v>
       </c>
       <c r="G15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.17934</v>
       </c>
       <c r="H15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20222999999999999</v>
       </c>
       <c r="I15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20222999999999999</v>
       </c>
       <c r="J15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20222999999999999</v>
       </c>
       <c r="K15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.20222999999999999</v>
       </c>
       <c r="L15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.18257399999999999</v>
       </c>
       <c r="M15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.18257399999999999</v>
       </c>
       <c r="N15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.18257399999999999</v>
       </c>
       <c r="O15" s="52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0.18257399999999999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated imports, changed variable names, updated options workbook
</commit_message>
<xml_diff>
--- a/applications/master/data/national/master_input.xlsx
+++ b/applications/master/data/national/master_input.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C8C53AB1-FE9C-834D-9746-34B55C4FDC57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{88397023-1374-D345-8AE6-47E90C37A391}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="961" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="961" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5840" yWindow="-20380" windowWidth="25180" windowHeight="20380" firstSheet="3" activeTab="8" xr2:uid="{8134AA81-6886-574D-B0B8-2D6ABE96B998}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -20,17 +21,17 @@
     <sheet name="Breastfeeding distribution" sheetId="50" r:id="rId5"/>
     <sheet name="Time trends" sheetId="51" r:id="rId6"/>
     <sheet name="Fertility risks" sheetId="42" r:id="rId7"/>
-    <sheet name="Programs cost and coverage" sheetId="56" r:id="rId8"/>
-    <sheet name="IYCF cost" sheetId="57" r:id="rId9"/>
-    <sheet name="Program dependencies" sheetId="58" r:id="rId10"/>
-    <sheet name="Reference programs" sheetId="59" r:id="rId11"/>
-    <sheet name="IYCF packages" sheetId="55" r:id="rId12"/>
+    <sheet name="IYCF packages" sheetId="55" r:id="rId8"/>
+    <sheet name="Programs cost and coverage" sheetId="56" r:id="rId9"/>
+    <sheet name="IYCF cost" sheetId="57" r:id="rId10"/>
+    <sheet name="Program dependencies" sheetId="58" r:id="rId11"/>
+    <sheet name="Reference programs" sheetId="59" r:id="rId12"/>
     <sheet name="Incidence of conditions" sheetId="7" r:id="rId13"/>
     <sheet name="Programs target population" sheetId="21" r:id="rId14"/>
     <sheet name="Programs family planning" sheetId="54" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="abortion" localSheetId="11">'Baseline year population inputs'!$C$26</definedName>
+    <definedName name="abortion" localSheetId="7">'Baseline year population inputs'!$C$26</definedName>
     <definedName name="abortion">'Baseline year population inputs'!$C$29</definedName>
     <definedName name="famplan_unmet_need">'Baseline year population inputs'!$C$8</definedName>
     <definedName name="food_insecure">'Baseline year population inputs'!$C$3</definedName>
@@ -63,7 +64,7 @@
     <definedName name="preterm_AGA">'Baseline year population inputs'!$C$34</definedName>
     <definedName name="preterm_SGA">'Baseline year population inputs'!$C$33</definedName>
     <definedName name="school_attendance">'Baseline year population inputs'!$C$5</definedName>
-    <definedName name="stillbirth" localSheetId="11">'Baseline year population inputs'!$C$27</definedName>
+    <definedName name="stillbirth" localSheetId="7">'Baseline year population inputs'!$C$27</definedName>
     <definedName name="stillbirth">'Baseline year population inputs'!$C$30</definedName>
     <definedName name="term_AGA">'Baseline year population inputs'!$C$36</definedName>
     <definedName name="term_SGA">'Baseline year population inputs'!$C$35</definedName>
@@ -79,6 +80,59 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sam</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+If user wants this, it must be checked for </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>all populations</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> b/c they are all targetted at once.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -117,11 +171,44 @@
         </r>
       </text>
     </comment>
+    <comment ref="D52" authorId="0" shapeId="0" xr:uid="{B5BA2B1F-1220-A74E-AAD5-1179315D509D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Sam:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Would like to put formula in here to define cost outside of code</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -221,7 +308,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam</author>
@@ -272,59 +359,6 @@
           </rPr>
           <t xml:space="preserve">
 When one program cannot exceed cov of another</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Sam</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>Sam:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-If user wants this, it must be checked for </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>all populations</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> b/c they are all targetted at once.</t>
         </r>
       </text>
     </comment>
@@ -4591,9 +4625,10 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4967,6 +5002,139 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36538F24-64B7-8D4B-91C5-47DA6C823CAD}">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.6640625" style="100" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" style="100"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
+      <c r="A1" s="105" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="104" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="104" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="104" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="104" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="103" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="91">
+        <f>1.5*0.61</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D2" s="91">
+        <f>0.5*0.61</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E2" s="91">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="102"/>
+      <c r="B3" s="102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="91">
+        <f>1.5*0.61</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D3" s="91">
+        <f>0.5*0.61</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E3" s="91">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="102"/>
+      <c r="B4" s="102" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="91">
+        <f>1.5*0.61</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D4" s="91">
+        <f>0.5*0.61</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E4" s="91">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="102"/>
+      <c r="B5" s="102" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="91">
+        <f>1.5*0.61</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D5" s="91">
+        <f>0.5*0.61</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E5" s="91">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="102"/>
+      <c r="B6" s="102" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="91">
+        <f>1.5*0.61</f>
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="D6" s="91">
+        <f>0.5*0.61</f>
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E6" s="91">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="101"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3709DAA-7BE5-6D41-BA4B-D86E9C571FF9}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -4974,8 +5142,9 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5335,7 +5504,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAC88371-B962-4B4C-A5B4-EAF9442C2DF9}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -5345,6 +5514,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -5430,225 +5600,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA2E456-F1D6-2946-9CF2-AA41D316F6C1}">
-  <sheetPr>
-    <tabColor theme="7" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:E21"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="17" style="63" customWidth="1"/>
-    <col min="2" max="2" width="19.1640625" style="63" customWidth="1"/>
-    <col min="3" max="3" width="13.5" style="63" customWidth="1"/>
-    <col min="4" max="16384" width="11.5" style="63"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A1" s="85" t="s">
-        <v>224</v>
-      </c>
-      <c r="B1" s="87" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" s="87" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1" s="87" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="87" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="83" t="s">
-        <v>219</v>
-      </c>
-      <c r="B2" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="D2" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" s="86"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="77"/>
-      <c r="B3" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="80"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="78"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="77"/>
-      <c r="B4" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="78"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="77"/>
-      <c r="B5" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="78"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A6" s="77"/>
-      <c r="B6" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="78"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A7" s="77"/>
-      <c r="B7" s="76" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="80"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A9" s="85" t="s">
-        <v>218</v>
-      </c>
-      <c r="B9" s="84" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="81"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A10" s="77"/>
-      <c r="B10" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="D10" s="80" t="s">
-        <v>217</v>
-      </c>
-      <c r="E10" s="78"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A11" s="77"/>
-      <c r="B11" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="78"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A12" s="77"/>
-      <c r="B12" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="78"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A13" s="77"/>
-      <c r="B13" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="78"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A14" s="77"/>
-      <c r="B14" s="76" t="s">
-        <v>215</v>
-      </c>
-      <c r="C14" s="75"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="80"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="83" t="s">
-        <v>216</v>
-      </c>
-      <c r="B16" s="76" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="73"/>
-      <c r="D16" s="82"/>
-      <c r="E16" s="81"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A17" s="77"/>
-      <c r="B17" s="76" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="73"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="78"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="77"/>
-      <c r="B18" s="76" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="80"/>
-      <c r="E18" s="78"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A19" s="77"/>
-      <c r="B19" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="73"/>
-      <c r="D19" s="80"/>
-      <c r="E19" s="78"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A20" s="77"/>
-      <c r="B20" s="76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="73"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="78"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A21" s="77"/>
-      <c r="B21" s="76" t="s">
-        <v>215</v>
-      </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="74"/>
-      <c r="E21" s="73"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5662,6 +5613,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -5777,6 +5729,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="118" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8130,6 +8083,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8339,6 +8293,7 @@
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -8985,6 +8940,7 @@
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9637,6 +9593,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10062,6 +10019,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10195,6 +10153,7 @@
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10400,6 +10359,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -10559,14 +10519,237 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA2E456-F1D6-2946-9CF2-AA41D316F6C1}">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17" style="63" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" style="63" customWidth="1"/>
+    <col min="3" max="3" width="13.5" style="63" customWidth="1"/>
+    <col min="4" max="16384" width="11.5" style="63"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A1" s="85" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" s="87" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="87" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="87" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A2" s="83" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="86"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="77"/>
+      <c r="B3" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="78"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="77"/>
+      <c r="B4" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="80"/>
+      <c r="D4" s="80"/>
+      <c r="E4" s="78"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A5" s="77"/>
+      <c r="B5" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="78"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="77"/>
+      <c r="B6" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="78"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="77"/>
+      <c r="B7" s="76" t="s">
+        <v>215</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="80"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A9" s="85" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" s="84" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="81"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A10" s="77"/>
+      <c r="B10" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="80" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="78"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A11" s="77"/>
+      <c r="B11" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80"/>
+      <c r="E11" s="78"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A12" s="77"/>
+      <c r="B12" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80"/>
+      <c r="E12" s="78"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A13" s="77"/>
+      <c r="B13" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="78"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A14" s="77"/>
+      <c r="B14" s="76" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="75"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="80"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="83" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="73"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="81"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A17" s="77"/>
+      <c r="B17" s="76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="73"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="78"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A18" s="77"/>
+      <c r="B18" s="76" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="73"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="78"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A19" s="77"/>
+      <c r="B19" s="76" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="73"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="78"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A20" s="77"/>
+      <c r="B20" s="76" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="73"/>
+      <c r="D20" s="79"/>
+      <c r="E20" s="78"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A21" s="77"/>
+      <c r="B21" s="76" t="s">
+        <v>215</v>
+      </c>
+      <c r="C21" s="75"/>
+      <c r="D21" s="74"/>
+      <c r="E21" s="73"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22549FF9-D8F2-7743-94EE-9F6E518F0245}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="1">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -11364,134 +11547,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36538F24-64B7-8D4B-91C5-47DA6C823CAD}">
-  <sheetPr>
-    <tabColor theme="7" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.6640625" style="100" customWidth="1"/>
-    <col min="2" max="16384" width="10.83203125" style="100"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" ht="40" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
-        <v>232</v>
-      </c>
-      <c r="B1" s="104" t="s">
-        <v>223</v>
-      </c>
-      <c r="C1" s="104" t="s">
-        <v>222</v>
-      </c>
-      <c r="D1" s="104" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="104" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="103" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="102" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="91">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D2" s="91">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E2" s="91">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="102"/>
-      <c r="B3" s="102" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="91">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D3" s="91">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E3" s="91">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="102"/>
-      <c r="B4" s="102" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="91">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D4" s="91">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E4" s="91">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="102"/>
-      <c r="B5" s="102" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="91">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D5" s="91">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E5" s="91">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="102"/>
-      <c r="B6" s="102" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="91">
-        <f>1.5*0.61</f>
-        <v>0.91500000000000004</v>
-      </c>
-      <c r="D6" s="91">
-        <f>0.5*0.61</f>
-        <v>0.30499999999999999</v>
-      </c>
-      <c r="E6" s="91">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="101"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed program from deps
</commit_message>
<xml_diff>
--- a/applications/master/data/national/master_input.xlsx
+++ b/applications/master/data/national/master_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samhainsworth/Desktop/github_projects/Nutrition/applications/master/data/national/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{625A1986-44A9-0D45-8419-8BE553C349B2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C12B0DB6-A500-FE4C-9E38-42AA5E0C23DB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35620" yWindow="-20300" windowWidth="27100" windowHeight="18820" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35620" yWindow="-20300" windowWidth="27100" windowHeight="18820" tabRatio="961" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Baseline year population inputs" sheetId="1" r:id="rId1"/>
@@ -486,7 +486,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="217">
   <si>
     <t>year</t>
   </si>
@@ -4514,7 +4514,7 @@
   </sheetPr>
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11:H12"/>
     </sheetView>
   </sheetViews>
@@ -5024,10 +5024,10 @@
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5051,39 +5051,33 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76" t="s">
-        <v>35</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="76"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="82" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="B3" s="76" t="s">
-        <v>60</v>
+        <v>161</v>
       </c>
       <c r="C3" s="76"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="82" t="s">
-        <v>59</v>
+        <v>162</v>
       </c>
       <c r="B4" s="76" t="s">
         <v>161</v>
       </c>
       <c r="C4" s="76"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="82" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="C5" s="76"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="52"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="52"/>
@@ -5105,9 +5099,6 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A17" s="52"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6536,47 +6527,47 @@
         <v>0</v>
       </c>
       <c r="E29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" ref="E29:O29" si="1">frac_maize</f>
         <v>0.05</v>
       </c>
       <c r="F29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="G29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="H29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="I29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="J29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="K29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="L29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="M29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="N29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
       <c r="O29" s="56">
-        <f>frac_maize</f>
+        <f t="shared" si="1"/>
         <v>0.05</v>
       </c>
     </row>
@@ -6591,47 +6582,47 @@
         <v>0</v>
       </c>
       <c r="E30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" ref="E30:O30" si="2">frac_rice</f>
         <v>0.8</v>
       </c>
       <c r="F30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="G30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="H30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="I30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="J30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="K30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="L30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="M30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="N30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
       <c r="O30" s="56">
-        <f>frac_rice</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
     </row>
@@ -6646,47 +6637,47 @@
         <v>0</v>
       </c>
       <c r="E31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" ref="E31:O31" si="3">frac_wheat</f>
         <v>0.12</v>
       </c>
       <c r="F31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="G31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="H31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="I31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="J31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="K31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="L31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="M31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="N31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
       <c r="O31" s="56">
-        <f>frac_wheat</f>
+        <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
     </row>
@@ -6739,55 +6730,55 @@
         <v>35</v>
       </c>
       <c r="C33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" ref="C33:O33" si="4">frac_malaria_risk</f>
         <v>0.1</v>
       </c>
       <c r="D33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="E33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="F33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="G33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="H33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="I33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="J33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="K33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="L33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="M33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="N33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
       <c r="O33" s="56">
-        <f>frac_malaria_risk</f>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
     </row>

</xml_diff>